<commit_message>
Added Select Company Feature ( DropDown With SearchBox ) , All Good !
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BE_SEM-1\Internship\invoice-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E24A24-8907-493F-ADAD-3F7FEDFB0824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6627064-488F-4150-8BF3-E224655F69EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>Tasks</t>
   </si>
   <si>
-    <t>Settings Page</t>
-  </si>
-  <si>
     <t>Company select input</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Settings Page add company add user</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,54 +427,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2">
         <v>4</v>
       </c>
       <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
       </c>
       <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -486,19 +486,19 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="5"/>
     </row>

</xml_diff>

<commit_message>
Added Taxation & JWT Auth
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -5,27 +5,36 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BE_SEM-1\Internship\invoice-generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BE_SEM-1\Internship\InvoiceApp\invoice-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6627064-488F-4150-8BF3-E224655F69EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8A7300-1A53-4BF1-A046-91D612CB2BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Tasks</t>
   </si>
@@ -58,13 +67,40 @@
   </si>
   <si>
     <t>Settings Page add company add user</t>
+  </si>
+  <si>
+    <t>Add Delete Button row to invoice table</t>
+  </si>
+  <si>
+    <t>invoice Table Item Desc col</t>
+  </si>
+  <si>
+    <t>User  Subscription</t>
+  </si>
+  <si>
+    <t>Display Registered Client &amp; Companies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save Draft Invoice </t>
+  </si>
+  <si>
+    <t>Copy Invoice  From History table</t>
+  </si>
+  <si>
+    <t>check duplicates when adding new Client / Company</t>
+  </si>
+  <si>
+    <t>Work on GUI</t>
+  </si>
+  <si>
+    <t>∞</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +111,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -119,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -130,6 +174,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,19 +457,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="37.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="47.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,8 +484,12 @@
       <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -446,9 +499,13 @@
       <c r="C2" s="2">
         <v>2</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2" s="3"/>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -459,8 +516,12 @@
         <v>3</v>
       </c>
       <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -472,7 +533,7 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -484,25 +545,86 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="5"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="2">
+        <f>AVERAGE(B2,B12)</f>
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>